<commit_message>
added incfrementally increasing house price
</commit_message>
<xml_diff>
--- a/calculation.xlsx
+++ b/calculation.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4047657\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4047657\Documents\calculations\hmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FF7EBF-8981-4A88-A8AA-99EDB2A015B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E449666-E8BB-431B-9E8F-2E3299FBB8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57765" yWindow="615" windowWidth="28755" windowHeight="14535" xr2:uid="{61E349DD-C396-4897-954F-94B6F0CC0F58}"/>
+    <workbookView xWindow="57645" yWindow="480" windowWidth="28755" windowHeight="14535" xr2:uid="{61E349DD-C396-4897-954F-94B6F0CC0F58}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
-    <sheet name="finance" sheetId="2" r:id="rId3"/>
+    <sheet name="finance" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Amount">finance!$B$4</definedName>
@@ -125,8 +124,8 @@
   <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="174" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -169,12 +168,12 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -265,49 +264,49 @@
             <c:strLit>
               <c:ptCount val="15"/>
               <c:pt idx="0">
-                <c:v>$1.00</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>$2.00</c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>$3.00</c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>$4.00</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>$5.00</c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>$6.00</c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>$7.00</c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>$8.00</c:v>
+                <c:v>8</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>$9.00</c:v>
+                <c:v>9</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>$10.00</c:v>
+                <c:v>10</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>$11.00</c:v>
+                <c:v>11</c:v>
               </c:pt>
               <c:pt idx="11">
-                <c:v>$12.00</c:v>
+                <c:v>12</c:v>
               </c:pt>
               <c:pt idx="12">
-                <c:v>$13.00</c:v>
+                <c:v>13</c:v>
               </c:pt>
               <c:pt idx="13">
-                <c:v>$14.00</c:v>
+                <c:v>14</c:v>
               </c:pt>
               <c:pt idx="14">
-                <c:v>$15.00</c:v>
+                <c:v>15</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -435,49 +434,49 @@
             <c:strLit>
               <c:ptCount val="15"/>
               <c:pt idx="0">
-                <c:v> 1 </c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v> 2 </c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v> 3 </c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v> 4 </c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v> 5 </c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v> 6 </c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v> 7 </c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v> 8 </c:v>
+                <c:v>8</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v> 9 </c:v>
+                <c:v>9</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v> 10 </c:v>
+                <c:v>10</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v> 11 </c:v>
+                <c:v>11</c:v>
               </c:pt>
               <c:pt idx="11">
-                <c:v> 12 </c:v>
+                <c:v>12</c:v>
               </c:pt>
               <c:pt idx="12">
-                <c:v> 13 </c:v>
+                <c:v>13</c:v>
               </c:pt>
               <c:pt idx="13">
-                <c:v> 14 </c:v>
+                <c:v>14</c:v>
               </c:pt>
               <c:pt idx="14">
-                <c:v> 15 </c:v>
+                <c:v>15</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -515,34 +514,34 @@
                   <c:v>2397194.017860794</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2853078.9244622998</c:v>
+                  <c:v>2359403.3802073235</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2806316.9254598962</c:v>
+                  <c:v>2319345.3042946449</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2756749.206517349</c:v>
+                  <c:v>2276883.7438272061</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2704207.4244382475</c:v>
+                  <c:v>2231874.4897317197</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2648513.1354344008</c:v>
+                  <c:v>2184164.6803905051</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2589477.1890903232</c:v>
+                  <c:v>2133592.2824888173</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2526899.0859656008</c:v>
+                  <c:v>2079985.5407130281</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2460566.2966533955</c:v>
+                  <c:v>2023162.3944306921</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2390253.5399824572</c:v>
+                  <c:v>1962929.8593714153</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2315722.0179112628</c:v>
+                  <c:v>1899083.3722085818</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -685,34 +684,34 @@
                   <c:v>679451.35248920647</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>438931.62181220111</c:v>
+                  <c:v>932607.16606717743</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>716134.35905381991</c:v>
+                  <c:v>1203105.9802190713</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1012273.6679123277</c:v>
+                  <c:v>1492139.1306024706</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1328647.051201507</c:v>
+                  <c:v>1800979.9859080347</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1666641.1535001365</c:v>
+                  <c:v>2130989.6085440321</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2027737.9000696321</c:v>
+                  <c:v>2483622.8066711379</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2413521.059435552</c:v>
+                  <c:v>2860434.6046881247</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2825683.2589258384</c:v>
+                  <c:v>3263087.1611485416</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3266033.4844873236</c:v>
+                  <c:v>3693357.1650983654</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3736505.0982714025</c:v>
+                  <c:v>4153143.7439740836</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -860,7 +859,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>main!$B$6</c15:sqref>
@@ -963,7 +962,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-636A-4FDA-948B-63E2418B118F}"/>
                   </c:ext>
@@ -976,7 +975,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>main!$C$6</c15:sqref>
@@ -1079,7 +1078,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-636A-4FDA-948B-63E2418B118F}"/>
                   </c:ext>
@@ -1092,7 +1091,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>main!$E$6</c15:sqref>
@@ -1201,7 +1200,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-636A-4FDA-948B-63E2418B118F}"/>
                   </c:ext>
@@ -1214,7 +1213,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>main!$F$6</c15:sqref>
@@ -1323,7 +1322,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-636A-4FDA-948B-63E2418B118F}"/>
                   </c:ext>
@@ -1336,7 +1335,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>main!$J$6</c15:sqref>
@@ -1412,40 +1411,40 @@
                         <c:v>507725.57621245563</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>309429.4733287929</c:v>
+                        <c:v>657451.25180863228</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>476270.24979811511</c:v>
+                        <c:v>800134.19058626681</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>635113.02243176207</c:v>
+                        <c:v>936186.55030322738</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>786424.14817987045</c:v>
+                        <c:v>1065997.2865072917</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>930643.71510626341</c:v>
+                        <c:v>1189933.4670713791</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>1068187.0305204827</c:v>
+                        <c:v>1308341.5123324799</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>1199446.0248873744</c:v>
+                        <c:v>1421548.3650454863</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>1324790.5762816588</c:v>
+                        <c:v>1529862.5941247847</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>1444569.7598850466</c:v>
+                        <c:v>1633575.4359215817</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>1559113.026768873</c:v>
+                        <c:v>1732961.7765727753</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-636A-4FDA-948B-63E2418B118F}"/>
                   </c:ext>
@@ -1462,6 +1461,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2544,8 +2544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBC43BD-A745-4AD3-8316-13267078B599}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2631,7 +2631,7 @@
         <v>500000</v>
       </c>
       <c r="D7" s="2">
-        <f>C7*(1+cap_appreciation_rate)</f>
+        <f t="shared" ref="D7:D26" si="0">C7*(1+cap_appreciation_rate)</f>
         <v>535000</v>
       </c>
       <c r="E7" s="3">
@@ -2639,7 +2639,7 @@
         <v>-36324.45574502361</v>
       </c>
       <c r="F7" s="7">
-        <f>C7*yield_rate</f>
+        <f t="shared" ref="F7:F26" si="1">C7*yield_rate</f>
         <v>20000</v>
       </c>
       <c r="G7" s="3">
@@ -2647,7 +2647,6 @@
         <v>-16324.45574502361</v>
       </c>
       <c r="H7" s="2">
-        <f>finance!Q9</f>
         <v>493675.54425497638</v>
       </c>
       <c r="I7" s="7">
@@ -2655,7 +2654,7 @@
         <v>41324.455745023617</v>
       </c>
       <c r="J7" s="7">
-        <f>I7/(1+inflation)^A7</f>
+        <f t="shared" ref="J7:J26" si="2">I7/(1+inflation)^A7</f>
         <v>38985.335608512847</v>
       </c>
     </row>
@@ -2671,7 +2670,7 @@
         <v>1035000</v>
       </c>
       <c r="D8" s="2">
-        <f>C8*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>1107450</v>
       </c>
       <c r="E8" s="3">
@@ -2679,23 +2678,22 @@
         <v>-72648.91149004722</v>
       </c>
       <c r="F8" s="7">
-        <f>C8*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>41400</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" ref="G8:G26" si="0">E8+F8</f>
+        <f t="shared" ref="G8:G26" si="3">E8+F8</f>
         <v>-31248.91149004722</v>
       </c>
       <c r="H8" s="2">
-        <f>finance!Q10</f>
         <v>980647.16542022768</v>
       </c>
       <c r="I8" s="7">
-        <f t="shared" ref="I8:I26" si="1">D8-H8</f>
+        <f t="shared" ref="I8:I26" si="4">D8-H8</f>
         <v>126802.83457977232</v>
       </c>
       <c r="J8" s="7">
-        <f>I8/(1+inflation)^A8</f>
+        <f t="shared" si="2"/>
         <v>112854.0713597119</v>
       </c>
     </row>
@@ -2707,11 +2705,11 @@
         <v>500000</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" ref="C9:C26" si="2">D8+B9</f>
+        <f t="shared" ref="C9:C26" si="5">D8+B9</f>
         <v>1607450</v>
       </c>
       <c r="D9" s="2">
-        <f>C9*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>1719971.5</v>
       </c>
       <c r="E9" s="3">
@@ -2719,23 +2717,22 @@
         <v>-108973.36723507082</v>
       </c>
       <c r="F9" s="7">
-        <f>C9*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>64298</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-44675.367235070822</v>
       </c>
       <c r="H9" s="2">
-        <f>finance!Q11</f>
         <v>1460512.6281103706</v>
       </c>
       <c r="I9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>259458.8718896294</v>
       </c>
       <c r="J9" s="7">
-        <f>I9/(1+inflation)^A9</f>
+        <f t="shared" si="2"/>
         <v>217846.67199234045</v>
       </c>
     </row>
@@ -2747,11 +2744,11 @@
         <v>500000</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2219971.5</v>
       </c>
       <c r="D10" s="2">
-        <f>C10*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>2375369.5050000004</v>
       </c>
       <c r="E10" s="3">
@@ -2759,23 +2756,22 @@
         <v>-145297.82298009444</v>
       </c>
       <c r="F10" s="7">
-        <f>C10*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>88798.86</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-56498.962980094439</v>
       </c>
       <c r="H10" s="2">
-        <f>finance!Q12</f>
         <v>1932845.5628168983</v>
       </c>
       <c r="I10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>442523.94218310202</v>
       </c>
       <c r="J10" s="7">
-        <f>I10/(1+inflation)^A10</f>
+        <f t="shared" si="2"/>
         <v>350520.41043434321</v>
       </c>
     </row>
@@ -2787,11 +2783,11 @@
         <v>500000</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2875369.5050000004</v>
       </c>
       <c r="D11" s="2">
-        <f>C11*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>3076645.3703500004</v>
       </c>
       <c r="E11" s="3">
@@ -2799,23 +2795,22 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F11" s="7">
-        <f>C11*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>115014.78020000002</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-66607.498525118033</v>
       </c>
       <c r="H11" s="2">
-        <f>finance!Q13</f>
         <v>2397194.017860794</v>
       </c>
       <c r="I11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>679451.35248920647</v>
       </c>
       <c r="J11" s="7">
-        <f>I11/(1+inflation)^A11</f>
+        <f t="shared" si="2"/>
         <v>507725.57621245563</v>
       </c>
     </row>
@@ -2827,11 +2822,11 @@
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3076645.3703500004</v>
       </c>
       <c r="D12" s="2">
-        <f>C12*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>3292010.5462745009</v>
       </c>
       <c r="E12" s="3">
@@ -2839,24 +2834,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F12" s="7">
-        <f>C12*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>123065.81481400003</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-58556.46391111803</v>
       </c>
       <c r="H12" s="2">
-        <f>finance!Q14</f>
-        <v>2853078.9244622998</v>
+        <v>2359403.3802073235</v>
       </c>
       <c r="I12" s="7">
-        <f t="shared" si="1"/>
-        <v>438931.62181220111</v>
+        <f t="shared" si="4"/>
+        <v>932607.16606717743</v>
       </c>
       <c r="J12" s="7">
-        <f>I12/(1+inflation)^A12</f>
-        <v>309429.4733287929</v>
+        <f t="shared" si="2"/>
+        <v>657451.25180863228</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -2867,11 +2861,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3292010.5462745009</v>
       </c>
       <c r="D13" s="2">
-        <f>C13*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>3522451.2845137161</v>
       </c>
       <c r="E13" s="3">
@@ -2879,24 +2873,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F13" s="7">
-        <f>C13*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>131680.42185098003</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-49941.85687413803</v>
       </c>
       <c r="H13" s="2">
-        <f>finance!Q15</f>
-        <v>2806316.9254598962</v>
+        <v>2319345.3042946449</v>
       </c>
       <c r="I13" s="7">
-        <f t="shared" si="1"/>
-        <v>716134.35905381991</v>
+        <f t="shared" si="4"/>
+        <v>1203105.9802190713</v>
       </c>
       <c r="J13" s="7">
-        <f>I13/(1+inflation)^A13</f>
-        <v>476270.24979811511</v>
+        <f t="shared" si="2"/>
+        <v>800134.19058626681</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -2907,11 +2900,11 @@
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3522451.2845137161</v>
       </c>
       <c r="D14" s="2">
-        <f>C14*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>3769022.8744296767</v>
       </c>
       <c r="E14" s="3">
@@ -2919,24 +2912,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F14" s="7">
-        <f>C14*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>140898.05138054866</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-40724.227344569401</v>
       </c>
       <c r="H14" s="2">
-        <f>finance!Q16</f>
-        <v>2756749.206517349</v>
+        <v>2276883.7438272061</v>
       </c>
       <c r="I14" s="7">
-        <f t="shared" si="1"/>
-        <v>1012273.6679123277</v>
+        <f t="shared" si="4"/>
+        <v>1492139.1306024706</v>
       </c>
       <c r="J14" s="7">
-        <f>I14/(1+inflation)^A14</f>
-        <v>635113.02243176207</v>
+        <f t="shared" si="2"/>
+        <v>936186.55030322738</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2947,11 +2939,11 @@
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3769022.8744296767</v>
       </c>
       <c r="D15" s="2">
-        <f>C15*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>4032854.4756397544</v>
       </c>
       <c r="E15" s="3">
@@ -2959,24 +2951,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F15" s="7">
-        <f>C15*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>150760.91497718706</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-30861.363747930998</v>
       </c>
       <c r="H15" s="2">
-        <f>finance!Q17</f>
-        <v>2704207.4244382475</v>
+        <v>2231874.4897317197</v>
       </c>
       <c r="I15" s="7">
-        <f t="shared" si="1"/>
-        <v>1328647.051201507</v>
+        <f t="shared" si="4"/>
+        <v>1800979.9859080347</v>
       </c>
       <c r="J15" s="7">
-        <f>I15/(1+inflation)^A15</f>
-        <v>786424.14817987045</v>
+        <f t="shared" si="2"/>
+        <v>1065997.2865072917</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2987,11 +2978,11 @@
         <v>0</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4032854.4756397544</v>
       </c>
       <c r="D16" s="2">
-        <f>C16*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>4315154.2889345372</v>
       </c>
       <c r="E16" s="3">
@@ -2999,24 +2990,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F16" s="7">
-        <f>C16*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>161314.17902559019</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-20308.099699527869</v>
       </c>
       <c r="H16" s="2">
-        <f>finance!Q18</f>
-        <v>2648513.1354344008</v>
+        <v>2184164.6803905051</v>
       </c>
       <c r="I16" s="7">
-        <f t="shared" si="1"/>
-        <v>1666641.1535001365</v>
+        <f t="shared" si="4"/>
+        <v>2130989.6085440321</v>
       </c>
       <c r="J16" s="7">
-        <f>I16/(1+inflation)^A16</f>
-        <v>930643.71510626341</v>
+        <f t="shared" si="2"/>
+        <v>1189933.4670713791</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3027,11 +3017,11 @@
         <v>0</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4315154.2889345372</v>
       </c>
       <c r="D17" s="2">
-        <f>C17*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>4617215.0891599553</v>
       </c>
       <c r="E17" s="3">
@@ -3039,24 +3029,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F17" s="7">
-        <f>C17*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>172606.17155738149</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-9016.107167736569</v>
       </c>
       <c r="H17" s="2">
-        <f>finance!Q19</f>
-        <v>2589477.1890903232</v>
+        <v>2133592.2824888173</v>
       </c>
       <c r="I17" s="7">
-        <f t="shared" si="1"/>
-        <v>2027737.9000696321</v>
+        <f t="shared" si="4"/>
+        <v>2483622.8066711379</v>
       </c>
       <c r="J17" s="7">
-        <f>I17/(1+inflation)^A17</f>
-        <v>1068187.0305204827</v>
+        <f t="shared" si="2"/>
+        <v>1308341.5123324799</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3067,11 +3056,11 @@
         <v>0</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4617215.0891599553</v>
       </c>
       <c r="D18" s="2">
-        <f>C18*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>4940420.1454011528</v>
       </c>
       <c r="E18" s="3">
@@ -3079,24 +3068,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F18" s="7">
-        <f>C18*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>184688.6035663982</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3066.3248412801477</v>
       </c>
       <c r="H18" s="2">
-        <f>finance!Q20</f>
-        <v>2526899.0859656008</v>
+        <v>2079985.5407130281</v>
       </c>
       <c r="I18" s="7">
-        <f t="shared" si="1"/>
-        <v>2413521.059435552</v>
+        <f t="shared" si="4"/>
+        <v>2860434.6046881247</v>
       </c>
       <c r="J18" s="7">
-        <f>I18/(1+inflation)^A18</f>
-        <v>1199446.0248873744</v>
+        <f t="shared" si="2"/>
+        <v>1421548.3650454863</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3107,11 +3095,11 @@
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4940420.1454011528</v>
       </c>
       <c r="D19" s="2">
-        <f>C19*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>5286249.5555792339</v>
       </c>
       <c r="E19" s="3">
@@ -3119,24 +3107,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F19" s="7">
-        <f>C19*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>197616.80581604611</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15994.527090928052</v>
       </c>
       <c r="H19" s="2">
-        <f>finance!Q21</f>
-        <v>2460566.2966533955</v>
+        <v>2023162.3944306921</v>
       </c>
       <c r="I19" s="7">
-        <f t="shared" si="1"/>
-        <v>2825683.2589258384</v>
+        <f t="shared" si="4"/>
+        <v>3263087.1611485416</v>
       </c>
       <c r="J19" s="7">
-        <f>I19/(1+inflation)^A19</f>
-        <v>1324790.5762816588</v>
+        <f t="shared" si="2"/>
+        <v>1529862.5941247847</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3147,11 +3134,11 @@
         <v>0</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5286249.5555792339</v>
       </c>
       <c r="D20" s="2">
-        <f>C20*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>5656287.0244697807</v>
       </c>
       <c r="E20" s="3">
@@ -3159,24 +3146,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F20" s="7">
-        <f>C20*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>211449.98222316935</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>29827.703498051298</v>
       </c>
       <c r="H20" s="2">
-        <f>finance!Q22</f>
-        <v>2390253.5399824572</v>
+        <v>1962929.8593714153</v>
       </c>
       <c r="I20" s="7">
-        <f t="shared" si="1"/>
-        <v>3266033.4844873236</v>
+        <f t="shared" si="4"/>
+        <v>3693357.1650983654</v>
       </c>
       <c r="J20" s="7">
-        <f>I20/(1+inflation)^A20</f>
-        <v>1444569.7598850466</v>
+        <f t="shared" si="2"/>
+        <v>1633575.4359215817</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -3187,11 +3173,11 @@
         <v>0</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5656287.0244697807</v>
       </c>
       <c r="D21" s="2">
-        <f>C21*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>6052227.1161826653</v>
       </c>
       <c r="E21" s="3">
@@ -3199,24 +3185,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F21" s="7">
-        <f>C21*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>226251.48097879122</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>44629.202253673167</v>
       </c>
       <c r="H21" s="2">
-        <f>finance!Q23</f>
-        <v>2315722.0179112628</v>
+        <v>1899083.3722085818</v>
       </c>
       <c r="I21" s="7">
-        <f t="shared" si="1"/>
-        <v>3736505.0982714025</v>
+        <f t="shared" si="4"/>
+        <v>4153143.7439740836</v>
       </c>
       <c r="J21" s="7">
-        <f>I21/(1+inflation)^A21</f>
-        <v>1559113.026768873</v>
+        <f t="shared" si="2"/>
+        <v>1732961.7765727753</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -3227,11 +3212,11 @@
         <v>0</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6052227.1161826653</v>
       </c>
       <c r="D22" s="2">
-        <f>C22*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>6475883.0143154524</v>
       </c>
       <c r="E22" s="3">
@@ -3239,24 +3224,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F22" s="7">
-        <f>C22*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>242089.08464730662</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>60466.805922188563</v>
       </c>
       <c r="H22" s="2">
-        <f>finance!Q24</f>
-        <v>2236718.604515797</v>
+        <v>1831406.0958159787</v>
       </c>
       <c r="I22" s="7">
-        <f t="shared" si="1"/>
-        <v>4239164.4097996559</v>
+        <f t="shared" si="4"/>
+        <v>4644476.9184994735</v>
       </c>
       <c r="J22" s="7">
-        <f>I22/(1+inflation)^A22</f>
-        <v>1668731.3159650895</v>
+        <f t="shared" si="2"/>
+        <v>1828281.0787570742</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -3267,11 +3251,11 @@
         <v>0</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6475883.0143154524</v>
       </c>
       <c r="D23" s="2">
-        <f>C23*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>6929194.8253175346</v>
       </c>
       <c r="E23" s="3">
@@ -3279,24 +3263,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F23" s="7">
-        <f>C23*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>259035.3205726181</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>77413.041847500048</v>
       </c>
       <c r="H23" s="2">
-        <f>finance!Q25</f>
-        <v>2152974.9863166027</v>
+        <v>1759668.1828398192</v>
       </c>
       <c r="I23" s="7">
-        <f t="shared" si="1"/>
-        <v>4776219.8390009319</v>
+        <f t="shared" si="4"/>
+        <v>5169526.6424777154</v>
       </c>
       <c r="J23" s="7">
-        <f>I23/(1+inflation)^A23</f>
-        <v>1773718.1036018305</v>
+        <f t="shared" si="2"/>
+        <v>1919778.2560052138</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -3307,11 +3290,11 @@
         <v>0</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6929194.8253175346</v>
       </c>
       <c r="D24" s="2">
-        <f>C24*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>7414238.4630897623</v>
       </c>
       <c r="E24" s="3">
@@ -3319,24 +3302,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F24" s="7">
-        <f>C24*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>277167.79301270138</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>95545.514287583326</v>
       </c>
       <c r="H24" s="2">
-        <f>finance!Q26</f>
-        <v>2064206.7510254574</v>
+        <v>1683625.9950850904</v>
       </c>
       <c r="I24" s="7">
-        <f t="shared" si="1"/>
-        <v>5350031.7120643053</v>
+        <f t="shared" si="4"/>
+        <v>5730612.4680046719</v>
       </c>
       <c r="J24" s="7">
-        <f>I24/(1+inflation)^A24</f>
-        <v>1874350.3926660763</v>
+        <f t="shared" si="2"/>
+        <v>2007684.4975330429</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -3347,11 +3329,11 @@
         <v>0</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7414238.4630897623</v>
       </c>
       <c r="D25" s="2">
-        <f>C25*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>7933235.1555060465</v>
       </c>
       <c r="E25" s="3">
@@ -3359,24 +3341,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F25" s="7">
-        <f>C25*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>296569.53852359048</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>114947.25979847243</v>
       </c>
       <c r="H25" s="2">
-        <f>finance!Q27</f>
-        <v>1970112.4216168432</v>
+        <v>1603021.2760650779</v>
       </c>
       <c r="I25" s="7">
-        <f t="shared" si="1"/>
-        <v>5963122.7338892035</v>
+        <f t="shared" si="4"/>
+        <v>6330213.8794409689</v>
       </c>
       <c r="J25" s="7">
-        <f>I25/(1+inflation)^A25</f>
-        <v>1970889.6467542346</v>
+        <f t="shared" si="2"/>
+        <v>2092218.0463981668</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -3387,11 +3368,11 @@
         <v>0</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7933235.1555060465</v>
       </c>
       <c r="D26" s="2">
-        <f>C26*(1+cap_appreciation_rate)</f>
+        <f t="shared" si="0"/>
         <v>8488561.6163914707</v>
       </c>
       <c r="E26" s="3">
@@ -3399,24 +3380,23 @@
         <v>-181622.27872511806</v>
       </c>
       <c r="F26" s="7">
-        <f>C26*yield_rate</f>
+        <f t="shared" si="1"/>
         <v>317329.40622024186</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>135707.1274951238</v>
       </c>
       <c r="H26" s="2">
-        <f>finance!Q28</f>
-        <v>1870372.4324437121</v>
+        <v>1517580.2739038644</v>
       </c>
       <c r="I26" s="7">
-        <f t="shared" si="1"/>
-        <v>6618189.1839477587</v>
+        <f t="shared" si="4"/>
+        <v>6970981.3424876062</v>
       </c>
       <c r="J26" s="7">
-        <f>I26/(1+inflation)^A26</f>
-        <v>2063582.6709812679</v>
+        <f t="shared" si="2"/>
+        <v>2173584.9336223369</v>
       </c>
     </row>
   </sheetData>
@@ -3430,23 +3410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61B4587-9613-484B-B664-10D0FD182E64}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA2527A-3BE5-4BA5-A375-284826528062}">
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA2527A-3BE5-4BA5-A375-284826528062}">
-  <dimension ref="A1:Q43"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="T44" sqref="T44"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9:P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3456,11 +3424,11 @@
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3468,7 +3436,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3476,7 +3444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3485,7 +3453,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3493,7 +3461,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3518,30 +3486,30 @@
       <c r="L8">
         <v>2</v>
       </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
       <c r="N8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O8">
-        <v>4</v>
-      </c>
-      <c r="P8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" ref="B9:B38" si="0">PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
         <v>-36324.45574502361</v>
       </c>
       <c r="C9" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A9,Years*Payments___Year,Amount)</f>
+        <f t="shared" ref="C9:C38" si="1">PPMT(Annual_Rate/Payments___Year,A9,Years*Payments___Year,Amount)</f>
         <v>-6324.4557450236143</v>
       </c>
       <c r="D9" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A9,Years*Payments___Year,Amount)</f>
+        <f t="shared" ref="D9:D38" si="2">IPMT(Annual_Rate/Payments___Year,A9,Years*Payments___Year,Amount)</f>
         <v>-30000.000000000004</v>
       </c>
       <c r="E9" s="4">
@@ -3563,26 +3531,25 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2">
-        <f>SUM(K9:P9)</f>
+      <c r="P9" s="2">
+        <f>SUM(K9:O9)</f>
         <v>493675.54425497638</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C10" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A10,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-6703.9230897250318</v>
       </c>
       <c r="D10" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A10,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-29620.532655298583</v>
       </c>
       <c r="E10" s="4">
@@ -3597,7 +3564,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" ref="K10:K38" si="0">E10</f>
+        <f t="shared" ref="K10:K38" si="3">E10</f>
         <v>486971.62116525136</v>
       </c>
       <c r="L10" s="2">
@@ -3607,45 +3574,44 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2">
-        <f t="shared" ref="Q10:Q43" si="1">SUM(K10:P10)</f>
+      <c r="P10" s="2">
+        <f>SUM(K10:O10)</f>
         <v>980647.16542022768</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C11" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A11,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-7106.1584751085329</v>
       </c>
       <c r="D11" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A11,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-29218.297269915078</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" ref="E11:E38" si="2">E10+C11</f>
+        <f t="shared" ref="E11:E38" si="4">E10+C11</f>
         <v>479865.4626901428</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F10:F38" si="3">B11/52</f>
+        <f t="shared" ref="F11:F38" si="5">B11/52</f>
         <v>-698.54722586583864</v>
       </c>
       <c r="J11" s="1">
         <v>3</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>479865.4626901428</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" ref="L11:L42" si="4">E10</f>
+        <f t="shared" ref="L11:L42" si="6">E10</f>
         <v>486971.62116525136</v>
       </c>
       <c r="M11" s="2">
@@ -3654,49 +3620,48 @@
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2">
-        <f t="shared" si="1"/>
+      <c r="P11" s="2">
+        <f>SUM(K11:O11)</f>
         <v>1460512.6281103706</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C12" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A12,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-7532.5279836150457</v>
       </c>
       <c r="D12" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A12,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-28791.927761408566</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>472332.93470652774</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J12" s="1">
         <v>4</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>472332.93470652774</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>479865.4626901428</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" ref="M12:M42" si="5">E10</f>
+        <f t="shared" ref="M12:M42" si="7">E10</f>
         <v>486971.62116525136</v>
       </c>
       <c r="N12" s="2">
@@ -3704,1595 +3669,1474 @@
         <v>493675.54425497638</v>
       </c>
       <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2">
-        <f t="shared" si="1"/>
+      <c r="P12" s="2">
+        <f>SUM(K12:O12)</f>
         <v>1932845.5628168983</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C13" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A13,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-7984.4796626319485</v>
       </c>
       <c r="D13" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A13,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-28339.976082391666</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>464348.45504389581</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J13" s="1">
         <v>5</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>464348.45504389581</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>472332.93470652774</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>479865.4626901428</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" ref="N13:N42" si="6">E10</f>
+        <f t="shared" ref="N13:N42" si="8">E10</f>
         <v>486971.62116525136</v>
       </c>
       <c r="O13" s="2">
         <f>E9</f>
         <v>493675.54425497638</v>
       </c>
-      <c r="Q13" s="2">
-        <f t="shared" si="1"/>
+      <c r="P13" s="2">
+        <f>SUM(K13:O13)</f>
         <v>2397194.017860794</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C14" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A14,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-8463.5484423898633</v>
       </c>
       <c r="D14" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A14,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-27860.90730263375</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>455884.90660150594</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J14" s="1">
         <v>6</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>455884.90660150594</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>464348.45504389581</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>472332.93470652774</v>
       </c>
       <c r="N14" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>479865.4626901428</v>
       </c>
       <c r="O14" s="2">
-        <f t="shared" ref="O14:O42" si="7">E10</f>
+        <f t="shared" ref="O14:O42" si="9">E10</f>
         <v>486971.62116525136</v>
       </c>
       <c r="P14" s="2">
-        <f>E9</f>
-        <v>493675.54425497638</v>
-      </c>
-      <c r="Q14" s="2">
-        <f t="shared" si="1"/>
-        <v>2853078.9244622998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K14:O14)</f>
+        <v>2359403.3802073235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C15" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A15,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-8971.3613489332565</v>
       </c>
       <c r="D15" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A15,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-27353.094396090357</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>446913.54525257269</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J15" s="1">
         <v>7</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>446913.54525257269</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>455884.90660150594</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>464348.45504389581</v>
       </c>
       <c r="N15" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>472332.93470652774</v>
       </c>
       <c r="O15" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>479865.4626901428</v>
       </c>
       <c r="P15" s="2">
-        <f t="shared" ref="P15:P43" si="8">E10</f>
-        <v>486971.62116525136</v>
-      </c>
-      <c r="Q15" s="2">
-        <f t="shared" si="1"/>
-        <v>2806316.9254598962</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K15:O15)</f>
+        <v>2319345.3042946449</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C16" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A16,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-9509.6430298692521</v>
       </c>
       <c r="D16" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A16,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-26814.812715154363</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>437403.90222270344</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J16" s="1">
         <v>8</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>437403.90222270344</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>446913.54525257269</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>455884.90660150594</v>
       </c>
       <c r="N16" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>464348.45504389581</v>
       </c>
       <c r="O16" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>472332.93470652774</v>
       </c>
       <c r="P16" s="2">
-        <f t="shared" si="8"/>
-        <v>479865.4626901428</v>
-      </c>
-      <c r="Q16" s="2">
-        <f t="shared" si="1"/>
-        <v>2756749.206517349</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K16:O16)</f>
+        <v>2276883.7438272061</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>9</v>
       </c>
       <c r="B17" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C17" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A17,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-10080.221611661404</v>
       </c>
       <c r="D17" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A17,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-26244.23413336221</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>427323.68061104201</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J17" s="1">
         <v>9</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>427323.68061104201</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>437403.90222270344</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>446913.54525257269</v>
       </c>
       <c r="N17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>455884.90660150594</v>
       </c>
       <c r="O17" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>464348.45504389581</v>
       </c>
       <c r="P17" s="2">
-        <f t="shared" si="8"/>
-        <v>472332.93470652774</v>
-      </c>
-      <c r="Q17" s="2">
-        <f t="shared" si="1"/>
-        <v>2704207.4244382475</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K17:O17)</f>
+        <v>2231874.4897317197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10</v>
       </c>
       <c r="B18" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C18" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A18,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-10685.034908361091</v>
       </c>
       <c r="D18" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A18,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-25639.420836662524</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>416638.64570268092</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J18" s="1">
         <v>10</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>416638.64570268092</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>427323.68061104201</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>437403.90222270344</v>
       </c>
       <c r="N18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>446913.54525257269</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>455884.90660150594</v>
       </c>
       <c r="P18" s="2">
-        <f t="shared" si="8"/>
-        <v>464348.45504389581</v>
-      </c>
-      <c r="Q18" s="2">
-        <f t="shared" si="1"/>
-        <v>2648513.1354344008</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K18:O18)</f>
+        <v>2184164.6803905051</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>11</v>
       </c>
       <c r="B19" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C19" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A19,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-11326.137002862755</v>
       </c>
       <c r="D19" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A19,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-24998.318742160856</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>405312.50869981817</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J19" s="1">
         <v>11</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>405312.50869981817</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>416638.64570268092</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>427323.68061104201</v>
       </c>
       <c r="N19" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>437403.90222270344</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>446913.54525257269</v>
       </c>
       <c r="P19" s="2">
-        <f t="shared" si="8"/>
-        <v>455884.90660150594</v>
-      </c>
-      <c r="Q19" s="2">
-        <f t="shared" si="1"/>
-        <v>2589477.1890903232</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K19:O19)</f>
+        <v>2133592.2824888173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>12</v>
       </c>
       <c r="B20" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C20" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A20,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-12005.705223034522</v>
       </c>
       <c r="D20" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A20,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-24318.750521989092</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>393306.80347678362</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J20" s="1">
         <v>12</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>393306.80347678362</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>405312.50869981817</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>416638.64570268092</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>427323.68061104201</v>
       </c>
       <c r="O20" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>437403.90222270344</v>
       </c>
       <c r="P20" s="2">
-        <f t="shared" si="8"/>
-        <v>446913.54525257269</v>
-      </c>
-      <c r="Q20" s="2">
-        <f t="shared" si="1"/>
-        <v>2526899.0859656008</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K20:O20)</f>
+        <v>2079985.5407130281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>13</v>
       </c>
       <c r="B21" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C21" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A21,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-12726.047536416592</v>
       </c>
       <c r="D21" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A21,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-23598.408208607023</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>380580.755940367</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J21" s="1">
         <v>13</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>380580.755940367</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>393306.80347678362</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>405312.50869981817</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>416638.64570268092</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>427323.68061104201</v>
       </c>
       <c r="P21" s="2">
-        <f t="shared" si="8"/>
-        <v>437403.90222270344</v>
-      </c>
-      <c r="Q21" s="2">
-        <f t="shared" si="1"/>
-        <v>2460566.2966533955</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K21:O21)</f>
+        <v>2023162.3944306921</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>14</v>
       </c>
       <c r="B22" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C22" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A22,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-13489.610388601586</v>
       </c>
       <c r="D22" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A22,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-22834.845356422033</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>367091.1455517654</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J22" s="1">
         <v>14</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>367091.1455517654</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>380580.755940367</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>393306.80347678362</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>405312.50869981817</v>
       </c>
       <c r="O22" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>416638.64570268092</v>
       </c>
       <c r="P22" s="2">
-        <f t="shared" si="8"/>
-        <v>427323.68061104201</v>
-      </c>
-      <c r="Q22" s="2">
-        <f t="shared" si="1"/>
-        <v>2390253.5399824572</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K22:O22)</f>
+        <v>1962929.8593714153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>15</v>
       </c>
       <c r="B23" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C23" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A23,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-14298.987011917683</v>
       </c>
       <c r="D23" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A23,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-22025.468733105929</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>352792.1585398477</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J23" s="1">
         <v>15</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>352792.1585398477</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>367091.1455517654</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>380580.755940367</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>393306.80347678362</v>
       </c>
       <c r="O23" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>405312.50869981817</v>
       </c>
       <c r="P23" s="2">
-        <f t="shared" si="8"/>
-        <v>416638.64570268092</v>
-      </c>
-      <c r="Q23" s="2">
-        <f t="shared" si="1"/>
-        <v>2315722.0179112628</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K23:O23)</f>
+        <v>1899083.3722085818</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>16</v>
       </c>
       <c r="B24" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C24" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A24,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-15156.926232632744</v>
       </c>
       <c r="D24" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A24,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-21167.529512390873</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>337635.23230721499</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J24" s="1">
         <v>16</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>337635.23230721499</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>352792.1585398477</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>367091.1455517654</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>380580.755940367</v>
       </c>
       <c r="O24" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>393306.80347678362</v>
       </c>
       <c r="P24" s="2">
-        <f t="shared" si="8"/>
-        <v>405312.50869981817</v>
-      </c>
-      <c r="Q24" s="2">
-        <f t="shared" si="1"/>
-        <v>2236718.604515797</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K24:O24)</f>
+        <v>1831406.0958159787</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>17</v>
       </c>
       <c r="B25" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C25" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A25,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-16066.341806590708</v>
       </c>
       <c r="D25" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A25,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-20258.113938432904</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>321568.89050062426</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J25" s="1">
         <v>17</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>321568.89050062426</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>337635.23230721499</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>352792.1585398477</v>
       </c>
       <c r="N25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>367091.1455517654</v>
       </c>
       <c r="O25" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>380580.755940367</v>
       </c>
       <c r="P25" s="2">
-        <f t="shared" si="8"/>
-        <v>393306.80347678362</v>
-      </c>
-      <c r="Q25" s="2">
-        <f t="shared" si="1"/>
-        <v>2152974.9863166027</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K25:O25)</f>
+        <v>1759668.1828398192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>18</v>
       </c>
       <c r="B26" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C26" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A26,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-17030.322314986151</v>
       </c>
       <c r="D26" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A26,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-19294.133430037466</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>304538.56818563811</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J26" s="1">
         <v>18</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>304538.56818563811</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>321568.89050062426</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>337635.23230721499</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>352792.1585398477</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>367091.1455517654</v>
       </c>
       <c r="P26" s="2">
-        <f t="shared" si="8"/>
-        <v>380580.755940367</v>
-      </c>
-      <c r="Q26" s="2">
-        <f t="shared" si="1"/>
-        <v>2064206.7510254574</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K26:O26)</f>
+        <v>1683625.9950850904</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>19</v>
       </c>
       <c r="B27" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C27" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A27,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-18052.141653885319</v>
       </c>
       <c r="D27" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A27,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-18272.314091138294</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>286486.4265317528</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J27" s="1">
         <v>19</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>286486.4265317528</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>304538.56818563811</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>321568.89050062426</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>337635.23230721499</v>
       </c>
       <c r="O27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>352792.1585398477</v>
       </c>
       <c r="P27" s="2">
-        <f t="shared" si="8"/>
-        <v>367091.1455517654</v>
-      </c>
-      <c r="Q27" s="2">
-        <f t="shared" si="1"/>
-        <v>1970112.4216168432</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K27:O27)</f>
+        <v>1603021.2760650779</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>20</v>
       </c>
       <c r="B28" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C28" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A28,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-19135.270153118439</v>
       </c>
       <c r="D28" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A28,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-17189.185591905174</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>267351.15637863439</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J28" s="1">
         <v>20</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>267351.15637863439</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>286486.4265317528</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>304538.56818563811</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>321568.89050062426</v>
       </c>
       <c r="O28" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>337635.23230721499</v>
       </c>
       <c r="P28" s="2">
-        <f t="shared" si="8"/>
-        <v>352792.1585398477</v>
-      </c>
-      <c r="Q28" s="2">
-        <f t="shared" si="1"/>
-        <v>1870372.4324437121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K28:O28)</f>
+        <v>1517580.2739038644</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>21</v>
       </c>
       <c r="B29" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C29" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A29,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-20283.386362305544</v>
       </c>
       <c r="D29" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A29,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-16041.069382718066</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>247067.77001632884</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J29" s="1">
         <v>21</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>247067.77001632884</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>267351.15637863439</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>286486.4265317528</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>304538.56818563811</v>
       </c>
       <c r="O29" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>321568.89050062426</v>
       </c>
       <c r="P29" s="2">
-        <f t="shared" si="8"/>
-        <v>337635.23230721499</v>
-      </c>
-      <c r="Q29" s="2">
-        <f t="shared" si="1"/>
-        <v>1764648.0439201933</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K29:O29)</f>
+        <v>1427012.8116129783</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>22</v>
       </c>
       <c r="B30" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C30" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A30,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-21500.389544043876</v>
       </c>
       <c r="D30" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A30,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-14824.066200979736</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>225567.38047228497</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J30" s="1">
         <v>22</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>225567.38047228497</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>247067.77001632884</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>267351.15637863439</v>
       </c>
       <c r="N30" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>286486.4265317528</v>
       </c>
       <c r="O30" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>304538.56818563811</v>
       </c>
       <c r="P30" s="2">
-        <f t="shared" si="8"/>
-        <v>321568.89050062426</v>
-      </c>
-      <c r="Q30" s="2">
-        <f t="shared" si="1"/>
-        <v>1652580.1920852633</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K30:O30)</f>
+        <v>1331011.3015846391</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>23</v>
       </c>
       <c r="B31" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C31" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A31,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-22790.41291668651</v>
       </c>
       <c r="D31" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A31,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-13534.042828337102</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>202776.96755559847</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J31" s="1">
         <v>23</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>202776.96755559847</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>225567.38047228497</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>247067.77001632884</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>267351.15637863439</v>
       </c>
       <c r="O31" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>286486.4265317528</v>
       </c>
       <c r="P31" s="2">
-        <f t="shared" si="8"/>
-        <v>304538.56818563811</v>
-      </c>
-      <c r="Q31" s="2">
-        <f t="shared" si="1"/>
-        <v>1533788.2691402375</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K31:O31)</f>
+        <v>1229249.7009545993</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>24</v>
       </c>
       <c r="B32" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C32" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A32,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-24157.837691687702</v>
       </c>
       <c r="D32" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A32,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-12166.618053335913</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>178619.12986391078</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J32" s="1">
         <v>24</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>178619.12986391078</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>202776.96755559847</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>225567.38047228497</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>247067.77001632884</v>
       </c>
       <c r="O32" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>267351.15637863439</v>
       </c>
       <c r="P32" s="2">
-        <f t="shared" si="8"/>
-        <v>286486.4265317528</v>
-      </c>
-      <c r="Q32" s="2">
-        <f t="shared" si="1"/>
-        <v>1407868.8308185104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K32:O32)</f>
+        <v>1121382.4042867576</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>25</v>
       </c>
       <c r="B33" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C33" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A33,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-25607.307953188963</v>
       </c>
       <c r="D33" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A33,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-10717.14779183465</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>153011.82191072183</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J33" s="1">
         <v>25</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>153011.82191072183</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>178619.12986391078</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>202776.96755559847</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>225567.38047228497</v>
       </c>
       <c r="O33" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>247067.77001632884</v>
       </c>
       <c r="P33" s="2">
-        <f t="shared" si="8"/>
-        <v>267351.15637863439</v>
-      </c>
-      <c r="Q33" s="2">
-        <f t="shared" si="1"/>
-        <v>1274394.2261974793</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K33:O33)</f>
+        <v>1007043.069818845</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>26</v>
       </c>
       <c r="B34" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C34" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A34,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-27143.746430380299</v>
       </c>
       <c r="D34" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A34,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-9180.7093146433144</v>
       </c>
       <c r="E34" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>125868.07548034153</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J34" s="1">
         <v>26</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>125868.07548034153</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>153011.82191072183</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>178619.12986391078</v>
       </c>
       <c r="N34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>202776.96755559847</v>
       </c>
       <c r="O34" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>225567.38047228497</v>
       </c>
       <c r="P34" s="2">
-        <f t="shared" si="8"/>
-        <v>247067.77001632884</v>
-      </c>
-      <c r="Q34" s="2">
-        <f t="shared" si="1"/>
-        <v>1132911.1452991865</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K34:O34)</f>
+        <v>885843.37528285757</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>27</v>
       </c>
       <c r="B35" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C35" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A35,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-28772.371216203119</v>
       </c>
       <c r="D35" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A35,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-7552.0845288204964</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>97095.704264138418</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J35" s="1">
         <v>27</v>
       </c>
       <c r="K35" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>97095.704264138418</v>
       </c>
       <c r="L35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>125868.07548034153</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>153011.82191072183</v>
       </c>
       <c r="N35" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>178619.12986391078</v>
       </c>
       <c r="O35" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>202776.96755559847</v>
       </c>
       <c r="P35" s="2">
-        <f t="shared" si="8"/>
-        <v>225567.38047228497</v>
-      </c>
-      <c r="Q35" s="2">
-        <f t="shared" si="1"/>
-        <v>982939.07954699604</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K35:O35)</f>
+        <v>757371.69907471107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>28</v>
       </c>
       <c r="B36" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C36" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A36,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-30498.713489175301</v>
       </c>
       <c r="D36" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A36,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-5825.7422558483086</v>
       </c>
       <c r="E36" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>66596.990774963109</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J36" s="1">
         <v>28</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>66596.990774963109</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>97095.704264138418</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>125868.07548034153</v>
       </c>
       <c r="N36" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>153011.82191072183</v>
       </c>
       <c r="O36" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>178619.12986391078</v>
       </c>
       <c r="P36" s="2">
-        <f t="shared" si="8"/>
-        <v>202776.96755559847</v>
-      </c>
-      <c r="Q36" s="2">
-        <f t="shared" si="1"/>
-        <v>823968.68984967412</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K36:O36)</f>
+        <v>621191.72229407565</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>29</v>
       </c>
       <c r="B37" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C37" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A37,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-32328.636298525824</v>
       </c>
       <c r="D37" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A37,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-3995.819446497791</v>
       </c>
       <c r="E37" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>34268.354476437285</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J37" s="1">
         <v>29</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>34268.354476437285</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>66596.990774963109</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>97095.704264138418</v>
       </c>
       <c r="N37" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>125868.07548034153</v>
       </c>
       <c r="O37" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>153011.82191072183</v>
       </c>
       <c r="P37" s="2">
-        <f t="shared" si="8"/>
-        <v>178619.12986391078</v>
-      </c>
-      <c r="Q37" s="2">
-        <f t="shared" si="1"/>
-        <v>655460.07677051297</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K37:O37)</f>
+        <v>476840.94690660218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>30</v>
       </c>
       <c r="B38" s="4">
-        <f>PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="0"/>
         <v>-36324.45574502361</v>
       </c>
       <c r="C38" s="4">
-        <f>PPMT(Annual_Rate/Payments___Year,A38,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="1"/>
         <v>-34268.354476437373</v>
       </c>
       <c r="D38" s="4">
-        <f>IPMT(Annual_Rate/Payments___Year,A38,Years*Payments___Year,Amount)</f>
+        <f t="shared" si="2"/>
         <v>-2056.101268586242</v>
       </c>
       <c r="E38" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-8.7311491370201111E-11</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-698.54722586583864</v>
       </c>
       <c r="J38" s="1">
         <v>30</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-8.7311491370201111E-11</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>34268.354476437285</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>66596.990774963109</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>97095.704264138418</v>
       </c>
       <c r="O38" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>125868.07548034153</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" si="8"/>
-        <v>153011.82191072183</v>
-      </c>
-      <c r="Q38" s="2">
-        <f t="shared" si="1"/>
-        <v>476840.94690660213</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K38:O38)</f>
+        <v>323829.12499588029</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J39" s="1">
         <v>31</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-8.7311491370201111E-11</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>34268.354476437285</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>66596.990774963109</v>
       </c>
       <c r="O39" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>97095.704264138418</v>
       </c>
       <c r="P39" s="2">
-        <f t="shared" si="8"/>
-        <v>125868.07548034153</v>
-      </c>
-      <c r="Q39" s="2">
-        <f t="shared" si="1"/>
-        <v>323829.12499588029</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K39:O39)</f>
+        <v>197961.04951553873</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J40" s="1">
         <v>32</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-8.7311491370201111E-11</v>
       </c>
       <c r="N40" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>34268.354476437285</v>
       </c>
       <c r="O40" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>66596.990774963109</v>
       </c>
       <c r="P40" s="2">
-        <f t="shared" si="8"/>
-        <v>97095.704264138418</v>
-      </c>
-      <c r="Q40" s="2">
-        <f t="shared" si="1"/>
-        <v>197961.04951553873</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K40:O40)</f>
+        <v>100865.34525140031</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J41" s="1">
         <v>33</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N41" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-8.7311491370201111E-11</v>
       </c>
       <c r="O41" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>34268.354476437285</v>
       </c>
       <c r="P41" s="2">
-        <f t="shared" si="8"/>
-        <v>66596.990774963109</v>
-      </c>
-      <c r="Q41" s="2">
-        <f t="shared" si="1"/>
-        <v>100865.34525140031</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K41:O41)</f>
+        <v>34268.354476437198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J42" s="1">
         <v>34</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M42" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N42" s="2">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="M42" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="O42" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-8.7311491370201111E-11</v>
       </c>
       <c r="P42" s="2">
-        <f t="shared" si="8"/>
-        <v>34268.354476437285</v>
-      </c>
-      <c r="Q42" s="2">
-        <f t="shared" si="1"/>
-        <v>34268.354476437198</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+        <f>SUM(K42:O42)</f>
+        <v>-8.7311491370201111E-11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J43" s="1">
         <v>35</v>
       </c>
       <c r="P43" s="2">
-        <f t="shared" si="8"/>
-        <v>-8.7311491370201111E-11</v>
-      </c>
-      <c r="Q43" s="2">
-        <f t="shared" si="1"/>
-        <v>-8.7311491370201111E-11</v>
+        <f>SUM(K43:O43)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added single home calculation
</commit_message>
<xml_diff>
--- a/calculation.xlsx
+++ b/calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4047657\Documents\calculations\hmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E449666-E8BB-431B-9E8F-2E3299FBB8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901966B7-A5C0-4B46-968D-281CA91383E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57645" yWindow="480" windowWidth="28755" windowHeight="14535" xr2:uid="{61E349DD-C396-4897-954F-94B6F0CC0F58}"/>
+    <workbookView xWindow="59745" yWindow="0" windowWidth="15870" windowHeight="14535" activeTab="1" xr2:uid="{61E349DD-C396-4897-954F-94B6F0CC0F58}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -604,49 +604,49 @@
             <c:strLit>
               <c:ptCount val="15"/>
               <c:pt idx="0">
-                <c:v> 1 </c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v> 2 </c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v> 3 </c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v> 4 </c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v> 5 </c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v> 6 </c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v> 7 </c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v> 8 </c:v>
+                <c:v>8</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v> 9 </c:v>
+                <c:v>9</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v> 10 </c:v>
+                <c:v>10</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v> 11 </c:v>
+                <c:v>11</c:v>
               </c:pt>
               <c:pt idx="11">
-                <c:v> 12 </c:v>
+                <c:v>12</c:v>
               </c:pt>
               <c:pt idx="12">
-                <c:v> 13 </c:v>
+                <c:v>13</c:v>
               </c:pt>
               <c:pt idx="13">
-                <c:v> 14 </c:v>
+                <c:v>14</c:v>
               </c:pt>
               <c:pt idx="14">
-                <c:v> 15 </c:v>
+                <c:v>15</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -2206,6 +2206,9 @@
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16BD5F98-5E5D-DEBE-6062-015DC7718A79}"/>
             </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
@@ -2544,8 +2547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBC43BD-A745-4AD3-8316-13267078B599}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3413,8 +3416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA2527A-3BE5-4BA5-A375-284826528062}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9:P41"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3532,7 +3535,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2">
-        <f>SUM(K9:O9)</f>
+        <f t="shared" ref="P9:P43" si="3">SUM(K9:O9)</f>
         <v>493675.54425497638</v>
       </c>
     </row>
@@ -3564,7 +3567,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" ref="K10:K38" si="3">E10</f>
+        <f t="shared" ref="K10:K38" si="4">E10</f>
         <v>486971.62116525136</v>
       </c>
       <c r="L10" s="2">
@@ -3575,7 +3578,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2">
-        <f>SUM(K10:O10)</f>
+        <f t="shared" si="3"/>
         <v>980647.16542022768</v>
       </c>
     </row>
@@ -3596,22 +3599,22 @@
         <v>-29218.297269915078</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" ref="E11:E38" si="4">E10+C11</f>
+        <f t="shared" ref="E11:E38" si="5">E10+C11</f>
         <v>479865.4626901428</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:F38" si="5">B11/52</f>
+        <f t="shared" ref="F11:F38" si="6">B11/52</f>
         <v>-698.54722586583864</v>
       </c>
       <c r="J11" s="1">
         <v>3</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>479865.4626901428</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" ref="L11:L42" si="6">E10</f>
+        <f t="shared" ref="L11:L42" si="7">E10</f>
         <v>486971.62116525136</v>
       </c>
       <c r="M11" s="2">
@@ -3621,7 +3624,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2">
-        <f>SUM(K11:O11)</f>
+        <f t="shared" si="3"/>
         <v>1460512.6281103706</v>
       </c>
     </row>
@@ -3642,26 +3645,26 @@
         <v>-28791.927761408566</v>
       </c>
       <c r="E12" s="4">
+        <f t="shared" si="5"/>
+        <v>472332.93470652774</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J12" s="1">
+        <v>4</v>
+      </c>
+      <c r="K12" s="2">
         <f t="shared" si="4"/>
         <v>472332.93470652774</v>
       </c>
-      <c r="F12" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J12" s="1">
-        <v>4</v>
-      </c>
-      <c r="K12" s="2">
-        <f t="shared" si="3"/>
-        <v>472332.93470652774</v>
-      </c>
       <c r="L12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>479865.4626901428</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" ref="M12:M42" si="7">E10</f>
+        <f t="shared" ref="M12:M42" si="8">E10</f>
         <v>486971.62116525136</v>
       </c>
       <c r="N12" s="2">
@@ -3670,7 +3673,7 @@
       </c>
       <c r="O12" s="2"/>
       <c r="P12" s="2">
-        <f>SUM(K12:O12)</f>
+        <f t="shared" si="3"/>
         <v>1932845.5628168983</v>
       </c>
     </row>
@@ -3691,30 +3694,30 @@
         <v>-28339.976082391666</v>
       </c>
       <c r="E13" s="4">
+        <f t="shared" si="5"/>
+        <v>464348.45504389581</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J13" s="1">
+        <v>5</v>
+      </c>
+      <c r="K13" s="2">
         <f t="shared" si="4"/>
         <v>464348.45504389581</v>
       </c>
-      <c r="F13" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J13" s="1">
-        <v>5</v>
-      </c>
-      <c r="K13" s="2">
-        <f t="shared" si="3"/>
-        <v>464348.45504389581</v>
-      </c>
       <c r="L13" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>472332.93470652774</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479865.4626901428</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" ref="N13:N42" si="8">E10</f>
+        <f t="shared" ref="N13:N42" si="9">E10</f>
         <v>486971.62116525136</v>
       </c>
       <c r="O13" s="2">
@@ -3722,7 +3725,7 @@
         <v>493675.54425497638</v>
       </c>
       <c r="P13" s="2">
-        <f>SUM(K13:O13)</f>
+        <f t="shared" si="3"/>
         <v>2397194.017860794</v>
       </c>
     </row>
@@ -3743,38 +3746,38 @@
         <v>-27860.90730263375</v>
       </c>
       <c r="E14" s="4">
+        <f t="shared" si="5"/>
+        <v>455884.90660150594</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J14" s="1">
+        <v>6</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" si="4"/>
         <v>455884.90660150594</v>
       </c>
-      <c r="F14" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J14" s="1">
-        <v>6</v>
-      </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
+        <f t="shared" si="7"/>
+        <v>464348.45504389581</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="8"/>
+        <v>472332.93470652774</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="9"/>
+        <v>479865.4626901428</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" ref="O14:O42" si="10">E10</f>
+        <v>486971.62116525136</v>
+      </c>
+      <c r="P14" s="2">
         <f t="shared" si="3"/>
-        <v>455884.90660150594</v>
-      </c>
-      <c r="L14" s="2">
-        <f t="shared" si="6"/>
-        <v>464348.45504389581</v>
-      </c>
-      <c r="M14" s="2">
-        <f t="shared" si="7"/>
-        <v>472332.93470652774</v>
-      </c>
-      <c r="N14" s="2">
-        <f t="shared" si="8"/>
-        <v>479865.4626901428</v>
-      </c>
-      <c r="O14" s="2">
-        <f t="shared" ref="O14:O42" si="9">E10</f>
-        <v>486971.62116525136</v>
-      </c>
-      <c r="P14" s="2">
-        <f>SUM(K14:O14)</f>
         <v>2359403.3802073235</v>
       </c>
     </row>
@@ -3795,38 +3798,38 @@
         <v>-27353.094396090357</v>
       </c>
       <c r="E15" s="4">
+        <f t="shared" si="5"/>
+        <v>446913.54525257269</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J15" s="1">
+        <v>7</v>
+      </c>
+      <c r="K15" s="2">
         <f t="shared" si="4"/>
         <v>446913.54525257269</v>
       </c>
-      <c r="F15" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J15" s="1">
-        <v>7</v>
-      </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
+        <f t="shared" si="7"/>
+        <v>455884.90660150594</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="8"/>
+        <v>464348.45504389581</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="9"/>
+        <v>472332.93470652774</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="10"/>
+        <v>479865.4626901428</v>
+      </c>
+      <c r="P15" s="2">
         <f t="shared" si="3"/>
-        <v>446913.54525257269</v>
-      </c>
-      <c r="L15" s="2">
-        <f t="shared" si="6"/>
-        <v>455884.90660150594</v>
-      </c>
-      <c r="M15" s="2">
-        <f t="shared" si="7"/>
-        <v>464348.45504389581</v>
-      </c>
-      <c r="N15" s="2">
-        <f t="shared" si="8"/>
-        <v>472332.93470652774</v>
-      </c>
-      <c r="O15" s="2">
-        <f t="shared" si="9"/>
-        <v>479865.4626901428</v>
-      </c>
-      <c r="P15" s="2">
-        <f>SUM(K15:O15)</f>
         <v>2319345.3042946449</v>
       </c>
     </row>
@@ -3847,38 +3850,38 @@
         <v>-26814.812715154363</v>
       </c>
       <c r="E16" s="4">
+        <f t="shared" si="5"/>
+        <v>437403.90222270344</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J16" s="1">
+        <v>8</v>
+      </c>
+      <c r="K16" s="2">
         <f t="shared" si="4"/>
         <v>437403.90222270344</v>
       </c>
-      <c r="F16" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J16" s="1">
-        <v>8</v>
-      </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
+        <f t="shared" si="7"/>
+        <v>446913.54525257269</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="8"/>
+        <v>455884.90660150594</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="9"/>
+        <v>464348.45504389581</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="10"/>
+        <v>472332.93470652774</v>
+      </c>
+      <c r="P16" s="2">
         <f t="shared" si="3"/>
-        <v>437403.90222270344</v>
-      </c>
-      <c r="L16" s="2">
-        <f t="shared" si="6"/>
-        <v>446913.54525257269</v>
-      </c>
-      <c r="M16" s="2">
-        <f t="shared" si="7"/>
-        <v>455884.90660150594</v>
-      </c>
-      <c r="N16" s="2">
-        <f t="shared" si="8"/>
-        <v>464348.45504389581</v>
-      </c>
-      <c r="O16" s="2">
-        <f t="shared" si="9"/>
-        <v>472332.93470652774</v>
-      </c>
-      <c r="P16" s="2">
-        <f>SUM(K16:O16)</f>
         <v>2276883.7438272061</v>
       </c>
     </row>
@@ -3899,38 +3902,38 @@
         <v>-26244.23413336221</v>
       </c>
       <c r="E17" s="4">
+        <f t="shared" si="5"/>
+        <v>427323.68061104201</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J17" s="1">
+        <v>9</v>
+      </c>
+      <c r="K17" s="2">
         <f t="shared" si="4"/>
         <v>427323.68061104201</v>
       </c>
-      <c r="F17" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J17" s="1">
-        <v>9</v>
-      </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
+        <f t="shared" si="7"/>
+        <v>437403.90222270344</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="8"/>
+        <v>446913.54525257269</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="9"/>
+        <v>455884.90660150594</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="10"/>
+        <v>464348.45504389581</v>
+      </c>
+      <c r="P17" s="2">
         <f t="shared" si="3"/>
-        <v>427323.68061104201</v>
-      </c>
-      <c r="L17" s="2">
-        <f t="shared" si="6"/>
-        <v>437403.90222270344</v>
-      </c>
-      <c r="M17" s="2">
-        <f t="shared" si="7"/>
-        <v>446913.54525257269</v>
-      </c>
-      <c r="N17" s="2">
-        <f t="shared" si="8"/>
-        <v>455884.90660150594</v>
-      </c>
-      <c r="O17" s="2">
-        <f t="shared" si="9"/>
-        <v>464348.45504389581</v>
-      </c>
-      <c r="P17" s="2">
-        <f>SUM(K17:O17)</f>
         <v>2231874.4897317197</v>
       </c>
     </row>
@@ -3951,38 +3954,38 @@
         <v>-25639.420836662524</v>
       </c>
       <c r="E18" s="4">
+        <f t="shared" si="5"/>
+        <v>416638.64570268092</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J18" s="1">
+        <v>10</v>
+      </c>
+      <c r="K18" s="2">
         <f t="shared" si="4"/>
         <v>416638.64570268092</v>
       </c>
-      <c r="F18" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J18" s="1">
-        <v>10</v>
-      </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
+        <f t="shared" si="7"/>
+        <v>427323.68061104201</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="8"/>
+        <v>437403.90222270344</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="9"/>
+        <v>446913.54525257269</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="10"/>
+        <v>455884.90660150594</v>
+      </c>
+      <c r="P18" s="2">
         <f t="shared" si="3"/>
-        <v>416638.64570268092</v>
-      </c>
-      <c r="L18" s="2">
-        <f t="shared" si="6"/>
-        <v>427323.68061104201</v>
-      </c>
-      <c r="M18" s="2">
-        <f t="shared" si="7"/>
-        <v>437403.90222270344</v>
-      </c>
-      <c r="N18" s="2">
-        <f t="shared" si="8"/>
-        <v>446913.54525257269</v>
-      </c>
-      <c r="O18" s="2">
-        <f t="shared" si="9"/>
-        <v>455884.90660150594</v>
-      </c>
-      <c r="P18" s="2">
-        <f>SUM(K18:O18)</f>
         <v>2184164.6803905051</v>
       </c>
     </row>
@@ -4003,38 +4006,38 @@
         <v>-24998.318742160856</v>
       </c>
       <c r="E19" s="4">
+        <f t="shared" si="5"/>
+        <v>405312.50869981817</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J19" s="1">
+        <v>11</v>
+      </c>
+      <c r="K19" s="2">
         <f t="shared" si="4"/>
         <v>405312.50869981817</v>
       </c>
-      <c r="F19" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J19" s="1">
-        <v>11</v>
-      </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
+        <f t="shared" si="7"/>
+        <v>416638.64570268092</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="8"/>
+        <v>427323.68061104201</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="9"/>
+        <v>437403.90222270344</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="10"/>
+        <v>446913.54525257269</v>
+      </c>
+      <c r="P19" s="2">
         <f t="shared" si="3"/>
-        <v>405312.50869981817</v>
-      </c>
-      <c r="L19" s="2">
-        <f t="shared" si="6"/>
-        <v>416638.64570268092</v>
-      </c>
-      <c r="M19" s="2">
-        <f t="shared" si="7"/>
-        <v>427323.68061104201</v>
-      </c>
-      <c r="N19" s="2">
-        <f t="shared" si="8"/>
-        <v>437403.90222270344</v>
-      </c>
-      <c r="O19" s="2">
-        <f t="shared" si="9"/>
-        <v>446913.54525257269</v>
-      </c>
-      <c r="P19" s="2">
-        <f>SUM(K19:O19)</f>
         <v>2133592.2824888173</v>
       </c>
     </row>
@@ -4055,38 +4058,38 @@
         <v>-24318.750521989092</v>
       </c>
       <c r="E20" s="4">
+        <f t="shared" si="5"/>
+        <v>393306.80347678362</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J20" s="1">
+        <v>12</v>
+      </c>
+      <c r="K20" s="2">
         <f t="shared" si="4"/>
         <v>393306.80347678362</v>
       </c>
-      <c r="F20" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J20" s="1">
-        <v>12</v>
-      </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
+        <f t="shared" si="7"/>
+        <v>405312.50869981817</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="8"/>
+        <v>416638.64570268092</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="9"/>
+        <v>427323.68061104201</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="10"/>
+        <v>437403.90222270344</v>
+      </c>
+      <c r="P20" s="2">
         <f t="shared" si="3"/>
-        <v>393306.80347678362</v>
-      </c>
-      <c r="L20" s="2">
-        <f t="shared" si="6"/>
-        <v>405312.50869981817</v>
-      </c>
-      <c r="M20" s="2">
-        <f t="shared" si="7"/>
-        <v>416638.64570268092</v>
-      </c>
-      <c r="N20" s="2">
-        <f t="shared" si="8"/>
-        <v>427323.68061104201</v>
-      </c>
-      <c r="O20" s="2">
-        <f t="shared" si="9"/>
-        <v>437403.90222270344</v>
-      </c>
-      <c r="P20" s="2">
-        <f>SUM(K20:O20)</f>
         <v>2079985.5407130281</v>
       </c>
     </row>
@@ -4107,38 +4110,38 @@
         <v>-23598.408208607023</v>
       </c>
       <c r="E21" s="4">
+        <f t="shared" si="5"/>
+        <v>380580.755940367</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J21" s="1">
+        <v>13</v>
+      </c>
+      <c r="K21" s="2">
         <f t="shared" si="4"/>
         <v>380580.755940367</v>
       </c>
-      <c r="F21" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J21" s="1">
-        <v>13</v>
-      </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
+        <f t="shared" si="7"/>
+        <v>393306.80347678362</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="8"/>
+        <v>405312.50869981817</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="9"/>
+        <v>416638.64570268092</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="10"/>
+        <v>427323.68061104201</v>
+      </c>
+      <c r="P21" s="2">
         <f t="shared" si="3"/>
-        <v>380580.755940367</v>
-      </c>
-      <c r="L21" s="2">
-        <f t="shared" si="6"/>
-        <v>393306.80347678362</v>
-      </c>
-      <c r="M21" s="2">
-        <f t="shared" si="7"/>
-        <v>405312.50869981817</v>
-      </c>
-      <c r="N21" s="2">
-        <f t="shared" si="8"/>
-        <v>416638.64570268092</v>
-      </c>
-      <c r="O21" s="2">
-        <f t="shared" si="9"/>
-        <v>427323.68061104201</v>
-      </c>
-      <c r="P21" s="2">
-        <f>SUM(K21:O21)</f>
         <v>2023162.3944306921</v>
       </c>
     </row>
@@ -4159,38 +4162,38 @@
         <v>-22834.845356422033</v>
       </c>
       <c r="E22" s="4">
+        <f t="shared" si="5"/>
+        <v>367091.1455517654</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J22" s="1">
+        <v>14</v>
+      </c>
+      <c r="K22" s="2">
         <f t="shared" si="4"/>
         <v>367091.1455517654</v>
       </c>
-      <c r="F22" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J22" s="1">
-        <v>14</v>
-      </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
+        <f t="shared" si="7"/>
+        <v>380580.755940367</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="8"/>
+        <v>393306.80347678362</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="9"/>
+        <v>405312.50869981817</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="10"/>
+        <v>416638.64570268092</v>
+      </c>
+      <c r="P22" s="2">
         <f t="shared" si="3"/>
-        <v>367091.1455517654</v>
-      </c>
-      <c r="L22" s="2">
-        <f t="shared" si="6"/>
-        <v>380580.755940367</v>
-      </c>
-      <c r="M22" s="2">
-        <f t="shared" si="7"/>
-        <v>393306.80347678362</v>
-      </c>
-      <c r="N22" s="2">
-        <f t="shared" si="8"/>
-        <v>405312.50869981817</v>
-      </c>
-      <c r="O22" s="2">
-        <f t="shared" si="9"/>
-        <v>416638.64570268092</v>
-      </c>
-      <c r="P22" s="2">
-        <f>SUM(K22:O22)</f>
         <v>1962929.8593714153</v>
       </c>
     </row>
@@ -4211,38 +4214,38 @@
         <v>-22025.468733105929</v>
       </c>
       <c r="E23" s="4">
+        <f t="shared" si="5"/>
+        <v>352792.1585398477</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J23" s="1">
+        <v>15</v>
+      </c>
+      <c r="K23" s="2">
         <f t="shared" si="4"/>
         <v>352792.1585398477</v>
       </c>
-      <c r="F23" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J23" s="1">
-        <v>15</v>
-      </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
+        <f t="shared" si="7"/>
+        <v>367091.1455517654</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="8"/>
+        <v>380580.755940367</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="9"/>
+        <v>393306.80347678362</v>
+      </c>
+      <c r="O23" s="2">
+        <f t="shared" si="10"/>
+        <v>405312.50869981817</v>
+      </c>
+      <c r="P23" s="2">
         <f t="shared" si="3"/>
-        <v>352792.1585398477</v>
-      </c>
-      <c r="L23" s="2">
-        <f t="shared" si="6"/>
-        <v>367091.1455517654</v>
-      </c>
-      <c r="M23" s="2">
-        <f t="shared" si="7"/>
-        <v>380580.755940367</v>
-      </c>
-      <c r="N23" s="2">
-        <f t="shared" si="8"/>
-        <v>393306.80347678362</v>
-      </c>
-      <c r="O23" s="2">
-        <f t="shared" si="9"/>
-        <v>405312.50869981817</v>
-      </c>
-      <c r="P23" s="2">
-        <f>SUM(K23:O23)</f>
         <v>1899083.3722085818</v>
       </c>
     </row>
@@ -4263,38 +4266,38 @@
         <v>-21167.529512390873</v>
       </c>
       <c r="E24" s="4">
+        <f t="shared" si="5"/>
+        <v>337635.23230721499</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J24" s="1">
+        <v>16</v>
+      </c>
+      <c r="K24" s="2">
         <f t="shared" si="4"/>
         <v>337635.23230721499</v>
       </c>
-      <c r="F24" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J24" s="1">
-        <v>16</v>
-      </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
+        <f t="shared" si="7"/>
+        <v>352792.1585398477</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="8"/>
+        <v>367091.1455517654</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="9"/>
+        <v>380580.755940367</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="10"/>
+        <v>393306.80347678362</v>
+      </c>
+      <c r="P24" s="2">
         <f t="shared" si="3"/>
-        <v>337635.23230721499</v>
-      </c>
-      <c r="L24" s="2">
-        <f t="shared" si="6"/>
-        <v>352792.1585398477</v>
-      </c>
-      <c r="M24" s="2">
-        <f t="shared" si="7"/>
-        <v>367091.1455517654</v>
-      </c>
-      <c r="N24" s="2">
-        <f t="shared" si="8"/>
-        <v>380580.755940367</v>
-      </c>
-      <c r="O24" s="2">
-        <f t="shared" si="9"/>
-        <v>393306.80347678362</v>
-      </c>
-      <c r="P24" s="2">
-        <f>SUM(K24:O24)</f>
         <v>1831406.0958159787</v>
       </c>
     </row>
@@ -4315,38 +4318,38 @@
         <v>-20258.113938432904</v>
       </c>
       <c r="E25" s="4">
+        <f t="shared" si="5"/>
+        <v>321568.89050062426</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J25" s="1">
+        <v>17</v>
+      </c>
+      <c r="K25" s="2">
         <f t="shared" si="4"/>
         <v>321568.89050062426</v>
       </c>
-      <c r="F25" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J25" s="1">
-        <v>17</v>
-      </c>
-      <c r="K25" s="2">
+      <c r="L25" s="2">
+        <f t="shared" si="7"/>
+        <v>337635.23230721499</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="8"/>
+        <v>352792.1585398477</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="9"/>
+        <v>367091.1455517654</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="10"/>
+        <v>380580.755940367</v>
+      </c>
+      <c r="P25" s="2">
         <f t="shared" si="3"/>
-        <v>321568.89050062426</v>
-      </c>
-      <c r="L25" s="2">
-        <f t="shared" si="6"/>
-        <v>337635.23230721499</v>
-      </c>
-      <c r="M25" s="2">
-        <f t="shared" si="7"/>
-        <v>352792.1585398477</v>
-      </c>
-      <c r="N25" s="2">
-        <f t="shared" si="8"/>
-        <v>367091.1455517654</v>
-      </c>
-      <c r="O25" s="2">
-        <f t="shared" si="9"/>
-        <v>380580.755940367</v>
-      </c>
-      <c r="P25" s="2">
-        <f>SUM(K25:O25)</f>
         <v>1759668.1828398192</v>
       </c>
     </row>
@@ -4367,38 +4370,38 @@
         <v>-19294.133430037466</v>
       </c>
       <c r="E26" s="4">
+        <f t="shared" si="5"/>
+        <v>304538.56818563811</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J26" s="1">
+        <v>18</v>
+      </c>
+      <c r="K26" s="2">
         <f t="shared" si="4"/>
         <v>304538.56818563811</v>
       </c>
-      <c r="F26" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J26" s="1">
-        <v>18</v>
-      </c>
-      <c r="K26" s="2">
+      <c r="L26" s="2">
+        <f t="shared" si="7"/>
+        <v>321568.89050062426</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="8"/>
+        <v>337635.23230721499</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="9"/>
+        <v>352792.1585398477</v>
+      </c>
+      <c r="O26" s="2">
+        <f t="shared" si="10"/>
+        <v>367091.1455517654</v>
+      </c>
+      <c r="P26" s="2">
         <f t="shared" si="3"/>
-        <v>304538.56818563811</v>
-      </c>
-      <c r="L26" s="2">
-        <f t="shared" si="6"/>
-        <v>321568.89050062426</v>
-      </c>
-      <c r="M26" s="2">
-        <f t="shared" si="7"/>
-        <v>337635.23230721499</v>
-      </c>
-      <c r="N26" s="2">
-        <f t="shared" si="8"/>
-        <v>352792.1585398477</v>
-      </c>
-      <c r="O26" s="2">
-        <f t="shared" si="9"/>
-        <v>367091.1455517654</v>
-      </c>
-      <c r="P26" s="2">
-        <f>SUM(K26:O26)</f>
         <v>1683625.9950850904</v>
       </c>
     </row>
@@ -4419,38 +4422,38 @@
         <v>-18272.314091138294</v>
       </c>
       <c r="E27" s="4">
+        <f t="shared" si="5"/>
+        <v>286486.4265317528</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J27" s="1">
+        <v>19</v>
+      </c>
+      <c r="K27" s="2">
         <f t="shared" si="4"/>
         <v>286486.4265317528</v>
       </c>
-      <c r="F27" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J27" s="1">
-        <v>19</v>
-      </c>
-      <c r="K27" s="2">
+      <c r="L27" s="2">
+        <f t="shared" si="7"/>
+        <v>304538.56818563811</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="8"/>
+        <v>321568.89050062426</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="9"/>
+        <v>337635.23230721499</v>
+      </c>
+      <c r="O27" s="2">
+        <f t="shared" si="10"/>
+        <v>352792.1585398477</v>
+      </c>
+      <c r="P27" s="2">
         <f t="shared" si="3"/>
-        <v>286486.4265317528</v>
-      </c>
-      <c r="L27" s="2">
-        <f t="shared" si="6"/>
-        <v>304538.56818563811</v>
-      </c>
-      <c r="M27" s="2">
-        <f t="shared" si="7"/>
-        <v>321568.89050062426</v>
-      </c>
-      <c r="N27" s="2">
-        <f t="shared" si="8"/>
-        <v>337635.23230721499</v>
-      </c>
-      <c r="O27" s="2">
-        <f t="shared" si="9"/>
-        <v>352792.1585398477</v>
-      </c>
-      <c r="P27" s="2">
-        <f>SUM(K27:O27)</f>
         <v>1603021.2760650779</v>
       </c>
     </row>
@@ -4471,38 +4474,38 @@
         <v>-17189.185591905174</v>
       </c>
       <c r="E28" s="4">
+        <f t="shared" si="5"/>
+        <v>267351.15637863439</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J28" s="1">
+        <v>20</v>
+      </c>
+      <c r="K28" s="2">
         <f t="shared" si="4"/>
         <v>267351.15637863439</v>
       </c>
-      <c r="F28" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J28" s="1">
-        <v>20</v>
-      </c>
-      <c r="K28" s="2">
+      <c r="L28" s="2">
+        <f t="shared" si="7"/>
+        <v>286486.4265317528</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="8"/>
+        <v>304538.56818563811</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="9"/>
+        <v>321568.89050062426</v>
+      </c>
+      <c r="O28" s="2">
+        <f t="shared" si="10"/>
+        <v>337635.23230721499</v>
+      </c>
+      <c r="P28" s="2">
         <f t="shared" si="3"/>
-        <v>267351.15637863439</v>
-      </c>
-      <c r="L28" s="2">
-        <f t="shared" si="6"/>
-        <v>286486.4265317528</v>
-      </c>
-      <c r="M28" s="2">
-        <f t="shared" si="7"/>
-        <v>304538.56818563811</v>
-      </c>
-      <c r="N28" s="2">
-        <f t="shared" si="8"/>
-        <v>321568.89050062426</v>
-      </c>
-      <c r="O28" s="2">
-        <f t="shared" si="9"/>
-        <v>337635.23230721499</v>
-      </c>
-      <c r="P28" s="2">
-        <f>SUM(K28:O28)</f>
         <v>1517580.2739038644</v>
       </c>
     </row>
@@ -4523,38 +4526,38 @@
         <v>-16041.069382718066</v>
       </c>
       <c r="E29" s="4">
+        <f t="shared" si="5"/>
+        <v>247067.77001632884</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J29" s="1">
+        <v>21</v>
+      </c>
+      <c r="K29" s="2">
         <f t="shared" si="4"/>
         <v>247067.77001632884</v>
       </c>
-      <c r="F29" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J29" s="1">
-        <v>21</v>
-      </c>
-      <c r="K29" s="2">
+      <c r="L29" s="2">
+        <f t="shared" si="7"/>
+        <v>267351.15637863439</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="8"/>
+        <v>286486.4265317528</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="9"/>
+        <v>304538.56818563811</v>
+      </c>
+      <c r="O29" s="2">
+        <f t="shared" si="10"/>
+        <v>321568.89050062426</v>
+      </c>
+      <c r="P29" s="2">
         <f t="shared" si="3"/>
-        <v>247067.77001632884</v>
-      </c>
-      <c r="L29" s="2">
-        <f t="shared" si="6"/>
-        <v>267351.15637863439</v>
-      </c>
-      <c r="M29" s="2">
-        <f t="shared" si="7"/>
-        <v>286486.4265317528</v>
-      </c>
-      <c r="N29" s="2">
-        <f t="shared" si="8"/>
-        <v>304538.56818563811</v>
-      </c>
-      <c r="O29" s="2">
-        <f t="shared" si="9"/>
-        <v>321568.89050062426</v>
-      </c>
-      <c r="P29" s="2">
-        <f>SUM(K29:O29)</f>
         <v>1427012.8116129783</v>
       </c>
     </row>
@@ -4575,38 +4578,38 @@
         <v>-14824.066200979736</v>
       </c>
       <c r="E30" s="4">
+        <f t="shared" si="5"/>
+        <v>225567.38047228497</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J30" s="1">
+        <v>22</v>
+      </c>
+      <c r="K30" s="2">
         <f t="shared" si="4"/>
         <v>225567.38047228497</v>
       </c>
-      <c r="F30" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J30" s="1">
-        <v>22</v>
-      </c>
-      <c r="K30" s="2">
+      <c r="L30" s="2">
+        <f t="shared" si="7"/>
+        <v>247067.77001632884</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="8"/>
+        <v>267351.15637863439</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="9"/>
+        <v>286486.4265317528</v>
+      </c>
+      <c r="O30" s="2">
+        <f t="shared" si="10"/>
+        <v>304538.56818563811</v>
+      </c>
+      <c r="P30" s="2">
         <f t="shared" si="3"/>
-        <v>225567.38047228497</v>
-      </c>
-      <c r="L30" s="2">
-        <f t="shared" si="6"/>
-        <v>247067.77001632884</v>
-      </c>
-      <c r="M30" s="2">
-        <f t="shared" si="7"/>
-        <v>267351.15637863439</v>
-      </c>
-      <c r="N30" s="2">
-        <f t="shared" si="8"/>
-        <v>286486.4265317528</v>
-      </c>
-      <c r="O30" s="2">
-        <f t="shared" si="9"/>
-        <v>304538.56818563811</v>
-      </c>
-      <c r="P30" s="2">
-        <f>SUM(K30:O30)</f>
         <v>1331011.3015846391</v>
       </c>
     </row>
@@ -4627,38 +4630,38 @@
         <v>-13534.042828337102</v>
       </c>
       <c r="E31" s="4">
+        <f t="shared" si="5"/>
+        <v>202776.96755559847</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J31" s="1">
+        <v>23</v>
+      </c>
+      <c r="K31" s="2">
         <f t="shared" si="4"/>
         <v>202776.96755559847</v>
       </c>
-      <c r="F31" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J31" s="1">
-        <v>23</v>
-      </c>
-      <c r="K31" s="2">
+      <c r="L31" s="2">
+        <f t="shared" si="7"/>
+        <v>225567.38047228497</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="8"/>
+        <v>247067.77001632884</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="9"/>
+        <v>267351.15637863439</v>
+      </c>
+      <c r="O31" s="2">
+        <f t="shared" si="10"/>
+        <v>286486.4265317528</v>
+      </c>
+      <c r="P31" s="2">
         <f t="shared" si="3"/>
-        <v>202776.96755559847</v>
-      </c>
-      <c r="L31" s="2">
-        <f t="shared" si="6"/>
-        <v>225567.38047228497</v>
-      </c>
-      <c r="M31" s="2">
-        <f t="shared" si="7"/>
-        <v>247067.77001632884</v>
-      </c>
-      <c r="N31" s="2">
-        <f t="shared" si="8"/>
-        <v>267351.15637863439</v>
-      </c>
-      <c r="O31" s="2">
-        <f t="shared" si="9"/>
-        <v>286486.4265317528</v>
-      </c>
-      <c r="P31" s="2">
-        <f>SUM(K31:O31)</f>
         <v>1229249.7009545993</v>
       </c>
     </row>
@@ -4679,38 +4682,38 @@
         <v>-12166.618053335913</v>
       </c>
       <c r="E32" s="4">
+        <f t="shared" si="5"/>
+        <v>178619.12986391078</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J32" s="1">
+        <v>24</v>
+      </c>
+      <c r="K32" s="2">
         <f t="shared" si="4"/>
         <v>178619.12986391078</v>
       </c>
-      <c r="F32" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J32" s="1">
-        <v>24</v>
-      </c>
-      <c r="K32" s="2">
+      <c r="L32" s="2">
+        <f t="shared" si="7"/>
+        <v>202776.96755559847</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="8"/>
+        <v>225567.38047228497</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="9"/>
+        <v>247067.77001632884</v>
+      </c>
+      <c r="O32" s="2">
+        <f t="shared" si="10"/>
+        <v>267351.15637863439</v>
+      </c>
+      <c r="P32" s="2">
         <f t="shared" si="3"/>
-        <v>178619.12986391078</v>
-      </c>
-      <c r="L32" s="2">
-        <f t="shared" si="6"/>
-        <v>202776.96755559847</v>
-      </c>
-      <c r="M32" s="2">
-        <f t="shared" si="7"/>
-        <v>225567.38047228497</v>
-      </c>
-      <c r="N32" s="2">
-        <f t="shared" si="8"/>
-        <v>247067.77001632884</v>
-      </c>
-      <c r="O32" s="2">
-        <f t="shared" si="9"/>
-        <v>267351.15637863439</v>
-      </c>
-      <c r="P32" s="2">
-        <f>SUM(K32:O32)</f>
         <v>1121382.4042867576</v>
       </c>
     </row>
@@ -4731,38 +4734,38 @@
         <v>-10717.14779183465</v>
       </c>
       <c r="E33" s="4">
+        <f t="shared" si="5"/>
+        <v>153011.82191072183</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J33" s="1">
+        <v>25</v>
+      </c>
+      <c r="K33" s="2">
         <f t="shared" si="4"/>
         <v>153011.82191072183</v>
       </c>
-      <c r="F33" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J33" s="1">
-        <v>25</v>
-      </c>
-      <c r="K33" s="2">
+      <c r="L33" s="2">
+        <f t="shared" si="7"/>
+        <v>178619.12986391078</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="8"/>
+        <v>202776.96755559847</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="9"/>
+        <v>225567.38047228497</v>
+      </c>
+      <c r="O33" s="2">
+        <f t="shared" si="10"/>
+        <v>247067.77001632884</v>
+      </c>
+      <c r="P33" s="2">
         <f t="shared" si="3"/>
-        <v>153011.82191072183</v>
-      </c>
-      <c r="L33" s="2">
-        <f t="shared" si="6"/>
-        <v>178619.12986391078</v>
-      </c>
-      <c r="M33" s="2">
-        <f t="shared" si="7"/>
-        <v>202776.96755559847</v>
-      </c>
-      <c r="N33" s="2">
-        <f t="shared" si="8"/>
-        <v>225567.38047228497</v>
-      </c>
-      <c r="O33" s="2">
-        <f t="shared" si="9"/>
-        <v>247067.77001632884</v>
-      </c>
-      <c r="P33" s="2">
-        <f>SUM(K33:O33)</f>
         <v>1007043.069818845</v>
       </c>
     </row>
@@ -4783,38 +4786,38 @@
         <v>-9180.7093146433144</v>
       </c>
       <c r="E34" s="4">
+        <f t="shared" si="5"/>
+        <v>125868.07548034153</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J34" s="1">
+        <v>26</v>
+      </c>
+      <c r="K34" s="2">
         <f t="shared" si="4"/>
         <v>125868.07548034153</v>
       </c>
-      <c r="F34" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J34" s="1">
-        <v>26</v>
-      </c>
-      <c r="K34" s="2">
+      <c r="L34" s="2">
+        <f t="shared" si="7"/>
+        <v>153011.82191072183</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="8"/>
+        <v>178619.12986391078</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="9"/>
+        <v>202776.96755559847</v>
+      </c>
+      <c r="O34" s="2">
+        <f t="shared" si="10"/>
+        <v>225567.38047228497</v>
+      </c>
+      <c r="P34" s="2">
         <f t="shared" si="3"/>
-        <v>125868.07548034153</v>
-      </c>
-      <c r="L34" s="2">
-        <f t="shared" si="6"/>
-        <v>153011.82191072183</v>
-      </c>
-      <c r="M34" s="2">
-        <f t="shared" si="7"/>
-        <v>178619.12986391078</v>
-      </c>
-      <c r="N34" s="2">
-        <f t="shared" si="8"/>
-        <v>202776.96755559847</v>
-      </c>
-      <c r="O34" s="2">
-        <f t="shared" si="9"/>
-        <v>225567.38047228497</v>
-      </c>
-      <c r="P34" s="2">
-        <f>SUM(K34:O34)</f>
         <v>885843.37528285757</v>
       </c>
     </row>
@@ -4835,38 +4838,38 @@
         <v>-7552.0845288204964</v>
       </c>
       <c r="E35" s="4">
+        <f t="shared" si="5"/>
+        <v>97095.704264138418</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J35" s="1">
+        <v>27</v>
+      </c>
+      <c r="K35" s="2">
         <f t="shared" si="4"/>
         <v>97095.704264138418</v>
       </c>
-      <c r="F35" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J35" s="1">
-        <v>27</v>
-      </c>
-      <c r="K35" s="2">
+      <c r="L35" s="2">
+        <f t="shared" si="7"/>
+        <v>125868.07548034153</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="8"/>
+        <v>153011.82191072183</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="9"/>
+        <v>178619.12986391078</v>
+      </c>
+      <c r="O35" s="2">
+        <f t="shared" si="10"/>
+        <v>202776.96755559847</v>
+      </c>
+      <c r="P35" s="2">
         <f t="shared" si="3"/>
-        <v>97095.704264138418</v>
-      </c>
-      <c r="L35" s="2">
-        <f t="shared" si="6"/>
-        <v>125868.07548034153</v>
-      </c>
-      <c r="M35" s="2">
-        <f t="shared" si="7"/>
-        <v>153011.82191072183</v>
-      </c>
-      <c r="N35" s="2">
-        <f t="shared" si="8"/>
-        <v>178619.12986391078</v>
-      </c>
-      <c r="O35" s="2">
-        <f t="shared" si="9"/>
-        <v>202776.96755559847</v>
-      </c>
-      <c r="P35" s="2">
-        <f>SUM(K35:O35)</f>
         <v>757371.69907471107</v>
       </c>
     </row>
@@ -4887,38 +4890,38 @@
         <v>-5825.7422558483086</v>
       </c>
       <c r="E36" s="4">
+        <f t="shared" si="5"/>
+        <v>66596.990774963109</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J36" s="1">
+        <v>28</v>
+      </c>
+      <c r="K36" s="2">
         <f t="shared" si="4"/>
         <v>66596.990774963109</v>
       </c>
-      <c r="F36" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J36" s="1">
-        <v>28</v>
-      </c>
-      <c r="K36" s="2">
+      <c r="L36" s="2">
+        <f t="shared" si="7"/>
+        <v>97095.704264138418</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="8"/>
+        <v>125868.07548034153</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="9"/>
+        <v>153011.82191072183</v>
+      </c>
+      <c r="O36" s="2">
+        <f t="shared" si="10"/>
+        <v>178619.12986391078</v>
+      </c>
+      <c r="P36" s="2">
         <f t="shared" si="3"/>
-        <v>66596.990774963109</v>
-      </c>
-      <c r="L36" s="2">
-        <f t="shared" si="6"/>
-        <v>97095.704264138418</v>
-      </c>
-      <c r="M36" s="2">
-        <f t="shared" si="7"/>
-        <v>125868.07548034153</v>
-      </c>
-      <c r="N36" s="2">
-        <f t="shared" si="8"/>
-        <v>153011.82191072183</v>
-      </c>
-      <c r="O36" s="2">
-        <f t="shared" si="9"/>
-        <v>178619.12986391078</v>
-      </c>
-      <c r="P36" s="2">
-        <f>SUM(K36:O36)</f>
         <v>621191.72229407565</v>
       </c>
     </row>
@@ -4939,38 +4942,38 @@
         <v>-3995.819446497791</v>
       </c>
       <c r="E37" s="4">
+        <f t="shared" si="5"/>
+        <v>34268.354476437285</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J37" s="1">
+        <v>29</v>
+      </c>
+      <c r="K37" s="2">
         <f t="shared" si="4"/>
         <v>34268.354476437285</v>
       </c>
-      <c r="F37" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J37" s="1">
-        <v>29</v>
-      </c>
-      <c r="K37" s="2">
+      <c r="L37" s="2">
+        <f t="shared" si="7"/>
+        <v>66596.990774963109</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="8"/>
+        <v>97095.704264138418</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="9"/>
+        <v>125868.07548034153</v>
+      </c>
+      <c r="O37" s="2">
+        <f t="shared" si="10"/>
+        <v>153011.82191072183</v>
+      </c>
+      <c r="P37" s="2">
         <f t="shared" si="3"/>
-        <v>34268.354476437285</v>
-      </c>
-      <c r="L37" s="2">
-        <f t="shared" si="6"/>
-        <v>66596.990774963109</v>
-      </c>
-      <c r="M37" s="2">
-        <f t="shared" si="7"/>
-        <v>97095.704264138418</v>
-      </c>
-      <c r="N37" s="2">
-        <f t="shared" si="8"/>
-        <v>125868.07548034153</v>
-      </c>
-      <c r="O37" s="2">
-        <f t="shared" si="9"/>
-        <v>153011.82191072183</v>
-      </c>
-      <c r="P37" s="2">
-        <f>SUM(K37:O37)</f>
         <v>476840.94690660218</v>
       </c>
     </row>
@@ -4991,38 +4994,38 @@
         <v>-2056.101268586242</v>
       </c>
       <c r="E38" s="4">
+        <f t="shared" si="5"/>
+        <v>-8.7311491370201111E-11</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="6"/>
+        <v>-698.54722586583864</v>
+      </c>
+      <c r="J38" s="1">
+        <v>30</v>
+      </c>
+      <c r="K38" s="2">
         <f t="shared" si="4"/>
         <v>-8.7311491370201111E-11</v>
       </c>
-      <c r="F38" s="1">
-        <f t="shared" si="5"/>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="J38" s="1">
-        <v>30</v>
-      </c>
-      <c r="K38" s="2">
+      <c r="L38" s="2">
+        <f t="shared" si="7"/>
+        <v>34268.354476437285</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="8"/>
+        <v>66596.990774963109</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="9"/>
+        <v>97095.704264138418</v>
+      </c>
+      <c r="O38" s="2">
+        <f t="shared" si="10"/>
+        <v>125868.07548034153</v>
+      </c>
+      <c r="P38" s="2">
         <f t="shared" si="3"/>
-        <v>-8.7311491370201111E-11</v>
-      </c>
-      <c r="L38" s="2">
-        <f t="shared" si="6"/>
-        <v>34268.354476437285</v>
-      </c>
-      <c r="M38" s="2">
-        <f t="shared" si="7"/>
-        <v>66596.990774963109</v>
-      </c>
-      <c r="N38" s="2">
-        <f t="shared" si="8"/>
-        <v>97095.704264138418</v>
-      </c>
-      <c r="O38" s="2">
-        <f t="shared" si="9"/>
-        <v>125868.07548034153</v>
-      </c>
-      <c r="P38" s="2">
-        <f>SUM(K38:O38)</f>
         <v>323829.12499588029</v>
       </c>
     </row>
@@ -5032,23 +5035,23 @@
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.7311491370201111E-11</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>34268.354476437285</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>66596.990774963109</v>
       </c>
       <c r="O39" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>97095.704264138418</v>
       </c>
       <c r="P39" s="2">
-        <f>SUM(K39:O39)</f>
+        <f t="shared" si="3"/>
         <v>197961.04951553873</v>
       </c>
     </row>
@@ -5058,23 +5061,23 @@
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-8.7311491370201111E-11</v>
       </c>
       <c r="N40" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>34268.354476437285</v>
       </c>
       <c r="O40" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>66596.990774963109</v>
       </c>
       <c r="P40" s="2">
-        <f>SUM(K40:O40)</f>
+        <f t="shared" si="3"/>
         <v>100865.34525140031</v>
       </c>
     </row>
@@ -5084,23 +5087,23 @@
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M41" s="2">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
+      <c r="M41" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N41" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-8.7311491370201111E-11</v>
       </c>
       <c r="O41" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>34268.354476437285</v>
       </c>
       <c r="P41" s="2">
-        <f>SUM(K41:O41)</f>
+        <f t="shared" si="3"/>
         <v>34268.354476437198</v>
       </c>
     </row>
@@ -5110,23 +5113,23 @@
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M42" s="2">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N42" s="2">
+      <c r="M42" s="2">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
+      <c r="N42" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="O42" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-8.7311491370201111E-11</v>
       </c>
       <c r="P42" s="2">
-        <f>SUM(K42:O42)</f>
+        <f t="shared" si="3"/>
         <v>-8.7311491370201111E-11</v>
       </c>
     </row>
@@ -5135,7 +5138,7 @@
         <v>35</v>
       </c>
       <c r="P43" s="2">
-        <f>SUM(K43:O43)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>